<commit_message>
Formalizing and Cleaning Up documentation
</commit_message>
<xml_diff>
--- a/output-files/Momentum_Strategy/high-quality-momentum/HQM_Recommended_trades.xlsx
+++ b/output-files/Momentum_Strategy/high-quality-momentum/HQM_Recommended_trades.xlsx
@@ -100,15 +100,15 @@
     <t>IRM</t>
   </si>
   <si>
+    <t>UNH</t>
+  </si>
+  <si>
     <t>JNPR</t>
   </si>
   <si>
     <t>COST</t>
   </si>
   <si>
-    <t>UNH</t>
-  </si>
-  <si>
     <t>DGX</t>
   </si>
   <si>
@@ -124,36 +124,36 @@
     <t>ORLY</t>
   </si>
   <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>ANTM</t>
+  </si>
+  <si>
     <t>LLY</t>
   </si>
   <si>
-    <t>ANTM</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
     <t>VMC</t>
   </si>
   <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>BRO</t>
+  </si>
+  <si>
     <t>SHW</t>
   </si>
   <si>
-    <t>BRO</t>
-  </si>
-  <si>
-    <t>CNC</t>
+    <t>SCHW</t>
+  </si>
+  <si>
+    <t>KEYS</t>
   </si>
   <si>
     <t>ORCL</t>
   </si>
   <si>
-    <t>SCHW</t>
-  </si>
-  <si>
-    <t>KEYS</t>
-  </si>
-  <si>
     <t>CF</t>
   </si>
   <si>
@@ -163,46 +163,46 @@
     <t>TER</t>
   </si>
   <si>
+    <t>ABBV</t>
+  </si>
+  <si>
+    <t>FTNT</t>
+  </si>
+  <si>
     <t>UDR</t>
   </si>
   <si>
-    <t>FTNT</t>
-  </si>
-  <si>
     <t>KR</t>
   </si>
   <si>
-    <t>ABBV</t>
-  </si>
-  <si>
     <t>MCK</t>
   </si>
   <si>
+    <t>DVN</t>
+  </si>
+  <si>
     <t>PFG</t>
   </si>
   <si>
     <t>INTU</t>
   </si>
   <si>
-    <t>DVN</t>
-  </si>
-  <si>
     <t>MSI</t>
   </si>
   <si>
+    <t>DLTR</t>
+  </si>
+  <si>
+    <t>TMO</t>
+  </si>
+  <si>
     <t>NVR</t>
   </si>
   <si>
-    <t>TMO</t>
-  </si>
-  <si>
-    <t>DLTR</t>
-  </si>
-  <si>
     <t>AOS</t>
   </si>
   <si>
-    <t>AAP</t>
+    <t>TSCO</t>
   </si>
 </sst>
 </file>
@@ -612,37 +612,37 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>61.88</v>
+        <v>60.42</v>
       </c>
       <c r="D2">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="E2">
-        <v>0.6617849422014273</v>
+        <v>0.6717184691992699</v>
       </c>
       <c r="F2">
         <v>0.9384920634920636</v>
       </c>
       <c r="G2">
-        <v>0.567986134836524</v>
+        <v>0.574087553366797</v>
       </c>
       <c r="H2">
         <v>0.996031746031746</v>
       </c>
       <c r="I2">
-        <v>0.371128829854344</v>
+        <v>0.376257897993077</v>
       </c>
       <c r="J2">
         <v>0.992063492063492</v>
       </c>
       <c r="K2">
-        <v>0.162316597635668</v>
+        <v>0.1612514788887922</v>
       </c>
       <c r="L2">
-        <v>0.994047619047619</v>
+        <v>0.992063492063492</v>
       </c>
       <c r="M2">
-        <v>0.9801587301587301</v>
+        <v>0.9796626984126984</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -653,37 +653,37 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>2038.37</v>
+        <v>2068.72</v>
       </c>
       <c r="D3">
         <v>9</v>
       </c>
       <c r="E3">
-        <v>0.7099540693473551</v>
+        <v>0.720218940292021</v>
       </c>
       <c r="F3">
-        <v>0.9563492063492063</v>
+        <v>0.9583333333333333</v>
       </c>
       <c r="G3">
-        <v>0.4446301684431929</v>
+        <v>0.4530907762176153</v>
       </c>
       <c r="H3">
-        <v>0.9761904761904762</v>
+        <v>0.9801587301587301</v>
       </c>
       <c r="I3">
-        <v>0.2553177463428586</v>
+        <v>0.2610119310470973</v>
       </c>
       <c r="J3">
-        <v>0.9623015873015873</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="K3">
-        <v>0.06486601674385821</v>
+        <v>0.06647378113289389</v>
       </c>
       <c r="L3">
-        <v>0.8888888888888888</v>
+        <v>0.8908730158730158</v>
       </c>
       <c r="M3">
-        <v>0.9459325396825397</v>
+        <v>0.9484126984126984</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -694,37 +694,37 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>166.94</v>
+        <v>161.65</v>
       </c>
       <c r="D4">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E4">
-        <v>0.6996469469087374</v>
+        <v>0.6903642328819332</v>
       </c>
       <c r="F4">
-        <v>0.9484126984126984</v>
+        <v>0.9503968253968255</v>
       </c>
       <c r="G4">
-        <v>0.369830871243267</v>
+        <v>0.3729193308968812</v>
       </c>
       <c r="H4">
-        <v>0.9563492063492063</v>
+        <v>0.9583333333333333</v>
       </c>
       <c r="I4">
-        <v>0.2525163491159873</v>
+        <v>0.2541150963913641</v>
       </c>
       <c r="J4">
-        <v>0.9603174603174603</v>
+        <v>0.9583333333333333</v>
       </c>
       <c r="K4">
-        <v>0.0773715692247524</v>
+        <v>0.07807978574412182</v>
       </c>
       <c r="L4">
         <v>0.9186507936507937</v>
       </c>
       <c r="M4">
-        <v>0.9459325396825397</v>
+        <v>0.9464285714285714</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -735,37 +735,37 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>215.37</v>
+        <v>224.09</v>
       </c>
       <c r="D5">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E5">
-        <v>1.000050198419399</v>
+        <v>1.011838589033717</v>
       </c>
       <c r="F5">
         <v>0.9781746031746031</v>
       </c>
       <c r="G5">
-        <v>0.3842607389210486</v>
+        <v>0.3752299195097301</v>
       </c>
       <c r="H5">
-        <v>0.9682539682539683</v>
+        <v>0.9623015873015873</v>
       </c>
       <c r="I5">
-        <v>0.2112150750608644</v>
+        <v>0.2074347176558292</v>
       </c>
       <c r="J5">
         <v>0.9384920634920636</v>
       </c>
       <c r="K5">
-        <v>0.06505056134563027</v>
+        <v>0.06559685549792733</v>
       </c>
       <c r="L5">
-        <v>0.8908730158730158</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="M5">
-        <v>0.9439484126984127</v>
+        <v>0.9419642857142857</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -776,37 +776,37 @@
         <v>16</v>
       </c>
       <c r="C6">
-        <v>37.07</v>
+        <v>37.41</v>
       </c>
       <c r="D6">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E6">
-        <v>0.5280261930211391</v>
+        <v>0.5454102527174026</v>
       </c>
       <c r="F6">
-        <v>0.8492063492063493</v>
+        <v>0.8591269841269842</v>
       </c>
       <c r="G6">
-        <v>0.2948618615687354</v>
+        <v>0.2934991078121863</v>
       </c>
       <c r="H6">
-        <v>0.9166666666666667</v>
+        <v>0.9146825396825397</v>
       </c>
       <c r="I6">
-        <v>0.3426738993371112</v>
+        <v>0.3451915069445467</v>
       </c>
       <c r="J6">
         <v>0.9880952380952381</v>
       </c>
       <c r="K6">
-        <v>0.1795222466037127</v>
+        <v>0.1784328595677188</v>
       </c>
       <c r="L6">
-        <v>0.998015873015873</v>
+        <v>0.996031746031746</v>
       </c>
       <c r="M6">
-        <v>0.9379960317460319</v>
+        <v>0.939484126984127</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -817,37 +817,37 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <v>230.02</v>
+        <v>221.1</v>
       </c>
       <c r="D7">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E7">
-        <v>0.8312632719569687</v>
+        <v>0.834179107443876</v>
       </c>
       <c r="F7">
-        <v>0.9682539682539683</v>
+        <v>0.9702380952380952</v>
       </c>
       <c r="G7">
-        <v>0.3262717997569195</v>
+        <v>0.3331687363843215</v>
       </c>
       <c r="H7">
-        <v>0.9365079365079364</v>
+        <v>0.9384920634920636</v>
       </c>
       <c r="I7">
-        <v>0.1813498087331685</v>
+        <v>0.182465929222107</v>
       </c>
       <c r="J7">
         <v>0.9126984126984127</v>
       </c>
       <c r="K7">
-        <v>0.08020116513231731</v>
+        <v>0.07953581761053961</v>
       </c>
       <c r="L7">
-        <v>0.9265873015873016</v>
+        <v>0.9246031746031745</v>
       </c>
       <c r="M7">
-        <v>0.9360119047619048</v>
+        <v>0.9365079365079365</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -858,37 +858,37 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>648.1799999999999</v>
+        <v>654.59</v>
       </c>
       <c r="D8">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8">
-        <v>0.502648874856965</v>
+        <v>0.5017016800009241</v>
       </c>
       <c r="F8">
-        <v>0.8293650793650794</v>
+        <v>0.8273809523809524</v>
       </c>
       <c r="G8">
-        <v>0.399642521260604</v>
+        <v>0.3984880143868432</v>
       </c>
       <c r="H8">
         <v>0.9722222222222223</v>
       </c>
       <c r="I8">
-        <v>0.2651060613727672</v>
+        <v>0.2662965387250283</v>
       </c>
       <c r="J8">
-        <v>0.9682539682539683</v>
+        <v>0.9662698412698413</v>
       </c>
       <c r="K8">
-        <v>0.1071249449966053</v>
+        <v>0.1088171449751263</v>
       </c>
       <c r="L8">
-        <v>0.9682539682539683</v>
+        <v>0.9702380952380952</v>
       </c>
       <c r="M8">
-        <v>0.9345238095238095</v>
+        <v>0.9340277777777778</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -899,34 +899,34 @@
         <v>19</v>
       </c>
       <c r="C9">
-        <v>62.88</v>
+        <v>64.95999999999999</v>
       </c>
       <c r="D9">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E9">
-        <v>0.6332821134430872</v>
+        <v>0.6326607181755297</v>
       </c>
       <c r="F9">
-        <v>0.9246031746031745</v>
+        <v>0.9226190476190476</v>
       </c>
       <c r="G9">
-        <v>0.328843496646373</v>
+        <v>0.3180230324679472</v>
       </c>
       <c r="H9">
-        <v>0.9384920634920636</v>
+        <v>0.9325396825396826</v>
       </c>
       <c r="I9">
-        <v>0.2647386174507175</v>
+        <v>0.2712190583671489</v>
       </c>
       <c r="J9">
-        <v>0.9662698412698413</v>
+        <v>0.9702380952380952</v>
       </c>
       <c r="K9">
-        <v>0.06773053812306094</v>
+        <v>0.0693624356995295</v>
       </c>
       <c r="L9">
-        <v>0.8948412698412699</v>
+        <v>0.8988095238095238</v>
       </c>
       <c r="M9">
         <v>0.9310515873015873</v>
@@ -940,37 +940,37 @@
         <v>20</v>
       </c>
       <c r="C10">
-        <v>84.75</v>
+        <v>85.83</v>
       </c>
       <c r="D10">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E10">
-        <v>1.482941449865174</v>
+        <v>1.52286537052459</v>
       </c>
       <c r="F10">
         <v>0.998015873015873</v>
       </c>
       <c r="G10">
-        <v>1.364451835034918</v>
+        <v>1.352204272238328</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>1.121973231329924</v>
+        <v>1.114869788709645</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.01282547300069455</v>
+        <v>0.01277013536109424</v>
       </c>
       <c r="L10">
-        <v>0.6746031746031745</v>
+        <v>0.6706349206349206</v>
       </c>
       <c r="M10">
-        <v>0.9181547619047619</v>
+        <v>0.9171626984126984</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -981,34 +981,34 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <v>138.54</v>
+        <v>139.34</v>
       </c>
       <c r="D11">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E11">
-        <v>0.9071964958651052</v>
+        <v>0.9089422998398815</v>
       </c>
       <c r="F11">
         <v>0.9742063492063493</v>
       </c>
       <c r="G11">
-        <v>0.5054945791532038</v>
+        <v>0.4906239450215465</v>
       </c>
       <c r="H11">
-        <v>0.9861111111111112</v>
+        <v>0.9841269841269842</v>
       </c>
       <c r="I11">
-        <v>0.524300307763108</v>
+        <v>0.520418413282333</v>
       </c>
       <c r="J11">
         <v>0.996031746031746</v>
       </c>
       <c r="K11">
-        <v>0.01911651892866858</v>
+        <v>0.01946454912543436</v>
       </c>
       <c r="L11">
-        <v>0.7063492063492063</v>
+        <v>0.7083333333333333</v>
       </c>
       <c r="M11">
         <v>0.9156746031746033</v>
@@ -1022,37 +1022,37 @@
         <v>22</v>
       </c>
       <c r="C12">
-        <v>402.58</v>
+        <v>400.06</v>
       </c>
       <c r="D12">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12">
-        <v>0.5287082059740762</v>
+        <v>0.5110774751489479</v>
       </c>
       <c r="F12">
-        <v>0.8511904761904762</v>
+        <v>0.8353174603174603</v>
       </c>
       <c r="G12">
-        <v>0.4274878527289502</v>
+        <v>0.4374278458356072</v>
       </c>
       <c r="H12">
         <v>0.9742063492063493</v>
       </c>
       <c r="I12">
-        <v>0.1867102105560021</v>
+        <v>0.187384586580418</v>
       </c>
       <c r="J12">
-        <v>0.9226190476190476</v>
+        <v>0.9246031746031745</v>
       </c>
       <c r="K12">
-        <v>0.07059956749331642</v>
+        <v>0.07179873683350305</v>
       </c>
       <c r="L12">
-        <v>0.9007936507936507</v>
+        <v>0.9067460317460317</v>
       </c>
       <c r="M12">
-        <v>0.9122023809523809</v>
+        <v>0.910218253968254</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1063,31 +1063,31 @@
         <v>23</v>
       </c>
       <c r="C13">
-        <v>20.44</v>
+        <v>19.93</v>
       </c>
       <c r="D13">
-        <v>959</v>
+        <v>983</v>
       </c>
       <c r="E13">
-        <v>1.248677463265698</v>
+        <v>1.244939671999217</v>
       </c>
       <c r="F13">
-        <v>0.9880952380952381</v>
+        <v>0.9900793650793651</v>
       </c>
       <c r="G13">
-        <v>0.3820498893600335</v>
+        <v>0.3760323600499796</v>
       </c>
       <c r="H13">
-        <v>0.9662698412698413</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="I13">
-        <v>0.4746925105394302</v>
+        <v>0.474894116802023</v>
       </c>
       <c r="J13">
         <v>0.994047619047619</v>
       </c>
       <c r="K13">
-        <v>0.01125360393143431</v>
+        <v>0.01081094961732811</v>
       </c>
       <c r="L13">
         <v>0.6646825396825397</v>
@@ -1104,37 +1104,37 @@
         <v>24</v>
       </c>
       <c r="C14">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E14">
-        <v>1.283938748166056</v>
+        <v>1.235089104556205</v>
       </c>
       <c r="F14">
-        <v>0.9900793650793651</v>
+        <v>0.9880952380952381</v>
       </c>
       <c r="G14">
-        <v>0.2882280006305783</v>
+        <v>0.2884484321013906</v>
       </c>
       <c r="H14">
-        <v>0.9126984126984127</v>
+        <v>0.9107142857142857</v>
       </c>
       <c r="I14">
-        <v>0.1337395314608161</v>
+        <v>0.1308926010173577</v>
       </c>
       <c r="J14">
-        <v>0.8333333333333333</v>
+        <v>0.8313492063492063</v>
       </c>
       <c r="K14">
-        <v>0.0566175374322369</v>
+        <v>0.05829151307255812</v>
       </c>
       <c r="L14">
-        <v>0.875</v>
+        <v>0.878968253968254</v>
       </c>
       <c r="M14">
-        <v>0.9027777777777778</v>
+        <v>0.902281746031746</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1145,37 +1145,37 @@
         <v>25</v>
       </c>
       <c r="C15">
-        <v>455.24</v>
+        <v>437.56</v>
       </c>
       <c r="D15">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E15">
-        <v>0.5951582155276973</v>
+        <v>0.5999510559920331</v>
       </c>
       <c r="F15">
         <v>0.8988095238095238</v>
       </c>
       <c r="G15">
-        <v>0.3085024598328047</v>
+        <v>0.3144083275836123</v>
       </c>
       <c r="H15">
-        <v>0.9246031746031745</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="I15">
-        <v>0.277922147585399</v>
+        <v>0.2806023994937442</v>
       </c>
       <c r="J15">
         <v>0.9722222222222223</v>
       </c>
       <c r="K15">
-        <v>0.03987863815182662</v>
+        <v>0.04141371525310836</v>
       </c>
       <c r="L15">
-        <v>0.8055555555555556</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="M15">
-        <v>0.9002976190476191</v>
+        <v>0.902281746031746</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1186,37 +1186,37 @@
         <v>26</v>
       </c>
       <c r="C16">
-        <v>362.1</v>
+        <v>367.74</v>
       </c>
       <c r="D16">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16">
-        <v>0.6374107594240104</v>
+        <v>0.638881256637634</v>
       </c>
       <c r="F16">
-        <v>0.9265873015873016</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="G16">
-        <v>0.2330099556925971</v>
+        <v>0.227478601904615</v>
       </c>
       <c r="H16">
-        <v>0.8253968253968255</v>
+        <v>0.8134920634920636</v>
       </c>
       <c r="I16">
-        <v>0.1778902783657514</v>
+        <v>0.1698659674909043</v>
       </c>
       <c r="J16">
-        <v>0.9067460317460317</v>
+        <v>0.8908730158730158</v>
       </c>
       <c r="K16">
-        <v>0.08496006624227018</v>
+        <v>0.08383001879267259</v>
       </c>
       <c r="L16">
         <v>0.9404761904761905</v>
       </c>
       <c r="M16">
-        <v>0.8998015873015873</v>
+        <v>0.8933531746031746</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1227,37 +1227,37 @@
         <v>27</v>
       </c>
       <c r="C17">
-        <v>51.49</v>
+        <v>51.51</v>
       </c>
       <c r="D17">
         <v>380</v>
       </c>
       <c r="E17">
-        <v>0.861484700604255</v>
+        <v>0.8612970108189307</v>
       </c>
       <c r="F17">
         <v>0.9722222222222223</v>
       </c>
       <c r="G17">
-        <v>0.1891895977312687</v>
+        <v>0.1884343045998181</v>
       </c>
       <c r="H17">
-        <v>0.744047619047619</v>
+        <v>0.746031746031746</v>
       </c>
       <c r="I17">
-        <v>0.1618727167773283</v>
+        <v>0.1570664001249575</v>
       </c>
       <c r="J17">
-        <v>0.873015873015873</v>
+        <v>0.8611111111111112</v>
       </c>
       <c r="K17">
-        <v>0.09750337111009039</v>
+        <v>0.09474296410232744</v>
       </c>
       <c r="L17">
-        <v>0.9603174603174603</v>
+        <v>0.9583333333333333</v>
       </c>
       <c r="M17">
-        <v>0.8874007936507937</v>
+        <v>0.8844246031746033</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1268,37 +1268,37 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <v>33.85</v>
+        <v>491.26</v>
       </c>
       <c r="D18">
-        <v>579</v>
+        <v>39</v>
       </c>
       <c r="E18">
-        <v>0.54863881751852</v>
+        <v>0.4816175324268653</v>
       </c>
       <c r="F18">
-        <v>0.8611111111111112</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="G18">
-        <v>0.2706869385325675</v>
+        <v>0.2638779788959533</v>
       </c>
       <c r="H18">
-        <v>0.8849206349206349</v>
+        <v>0.878968253968254</v>
       </c>
       <c r="I18">
-        <v>0.2233231039531359</v>
+        <v>0.1706720198398182</v>
       </c>
       <c r="J18">
-        <v>0.9503968253968255</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="K18">
-        <v>0.04774650031112621</v>
+        <v>0.09136832687979328</v>
       </c>
       <c r="L18">
-        <v>0.8492063492063493</v>
+        <v>0.9543650793650794</v>
       </c>
       <c r="M18">
-        <v>0.8864087301587302</v>
+        <v>0.8839285714285714</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1309,37 +1309,37 @@
         <v>29</v>
       </c>
       <c r="C19">
-        <v>561.3099999999999</v>
+        <v>34.65</v>
       </c>
       <c r="D19">
-        <v>34</v>
+        <v>565</v>
       </c>
       <c r="E19">
-        <v>0.5215142217205716</v>
+        <v>0.5467216102404566</v>
       </c>
       <c r="F19">
+        <v>0.8611111111111112</v>
+      </c>
+      <c r="G19">
+        <v>0.2735537375977283</v>
+      </c>
+      <c r="H19">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="I19">
+        <v>0.2140075517855191</v>
+      </c>
+      <c r="J19">
+        <v>0.9424603174603174</v>
+      </c>
+      <c r="K19">
+        <v>0.04622534110540472</v>
+      </c>
+      <c r="L19">
         <v>0.8412698412698413</v>
       </c>
-      <c r="G19">
-        <v>0.4536079133462709</v>
-      </c>
-      <c r="H19">
-        <v>0.9801587301587301</v>
-      </c>
-      <c r="I19">
-        <v>0.1964677374812689</v>
-      </c>
-      <c r="J19">
-        <v>0.9325396825396826</v>
-      </c>
-      <c r="K19">
-        <v>0.0354009159671828</v>
-      </c>
-      <c r="L19">
-        <v>0.7857142857142857</v>
-      </c>
       <c r="M19">
-        <v>0.8849206349206349</v>
+        <v>0.8834325396825397</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1350,37 +1350,37 @@
         <v>30</v>
       </c>
       <c r="C20">
-        <v>505.78</v>
+        <v>551.7</v>
       </c>
       <c r="D20">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E20">
-        <v>0.4652130947509125</v>
+        <v>0.5051610197810745</v>
       </c>
       <c r="F20">
-        <v>0.7936507936507937</v>
+        <v>0.8313492063492063</v>
       </c>
       <c r="G20">
-        <v>0.267955266288621</v>
+        <v>0.4478004495050898</v>
       </c>
       <c r="H20">
-        <v>0.882936507936508</v>
+        <v>0.9781746031746031</v>
       </c>
       <c r="I20">
-        <v>0.1709317948290809</v>
+        <v>0.2033199544486164</v>
       </c>
       <c r="J20">
-        <v>0.8908730158730158</v>
+        <v>0.9365079365079364</v>
       </c>
       <c r="K20">
-        <v>0.08765826729987307</v>
+        <v>0.03557313827754947</v>
       </c>
       <c r="L20">
-        <v>0.9484126984126984</v>
+        <v>0.7876984126984127</v>
       </c>
       <c r="M20">
-        <v>0.878968253968254</v>
+        <v>0.8834325396825397</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1391,37 +1391,37 @@
         <v>31</v>
       </c>
       <c r="C21">
-        <v>174.4</v>
+        <v>178.8</v>
       </c>
       <c r="D21">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E21">
-        <v>0.4437666028720802</v>
+        <v>0.4408834930916197</v>
       </c>
       <c r="F21">
         <v>0.7698412698412699</v>
       </c>
       <c r="G21">
-        <v>0.3540151994649312</v>
+        <v>0.3629180041669744</v>
       </c>
       <c r="H21">
-        <v>0.9503968253968255</v>
+        <v>0.9523809523809524</v>
       </c>
       <c r="I21">
-        <v>0.1140948431985209</v>
+        <v>0.1134541735089961</v>
       </c>
       <c r="J21">
-        <v>0.7876984126984127</v>
+        <v>0.7936507936507937</v>
       </c>
       <c r="K21">
-        <v>0.1600569416503309</v>
+        <v>0.1645836781947405</v>
       </c>
       <c r="L21">
-        <v>0.992063492063492</v>
+        <v>0.994047619047619</v>
       </c>
       <c r="M21">
-        <v>0.875</v>
+        <v>0.8774801587301587</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1432,34 +1432,34 @@
         <v>32</v>
       </c>
       <c r="C22">
-        <v>174.59</v>
+        <v>178.89</v>
       </c>
       <c r="D22">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E22">
-        <v>0.3619540225070202</v>
+        <v>0.3712038362439146</v>
       </c>
       <c r="F22">
-        <v>0.6785714285714286</v>
+        <v>0.6884920634920636</v>
       </c>
       <c r="G22">
-        <v>0.319418136822908</v>
+        <v>0.329908803000066</v>
       </c>
       <c r="H22">
-        <v>0.9305555555555556</v>
+        <v>0.9365079365079364</v>
       </c>
       <c r="I22">
-        <v>0.1785927768784717</v>
+        <v>0.1745023201059541</v>
       </c>
       <c r="J22">
-        <v>0.9087301587301587</v>
+        <v>0.9007936507936507</v>
       </c>
       <c r="K22">
-        <v>0.08786014299964613</v>
+        <v>0.08538344886303736</v>
       </c>
       <c r="L22">
-        <v>0.9503968253968255</v>
+        <v>0.9424603174603174</v>
       </c>
       <c r="M22">
         <v>0.8670634920634921</v>
@@ -1473,37 +1473,37 @@
         <v>33</v>
       </c>
       <c r="C23">
-        <v>103.95</v>
+        <v>102.25</v>
       </c>
       <c r="D23">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E23">
-        <v>0.4970956322205213</v>
+        <v>0.4888952950518031</v>
       </c>
       <c r="F23">
-        <v>0.8253968253968255</v>
+        <v>0.8214285714285714</v>
       </c>
       <c r="G23">
-        <v>0.24010884711564</v>
+        <v>0.2415789843415</v>
       </c>
       <c r="H23">
         <v>0.8392857142857143</v>
       </c>
       <c r="I23">
-        <v>0.1835052021243233</v>
+        <v>0.1831401163189879</v>
       </c>
       <c r="J23">
         <v>0.9146825396825397</v>
       </c>
       <c r="K23">
-        <v>0.055028805062565</v>
+        <v>0.052833854666202</v>
       </c>
       <c r="L23">
-        <v>0.873015873015873</v>
+        <v>0.869047619047619</v>
       </c>
       <c r="M23">
-        <v>0.8630952380952381</v>
+        <v>0.861111111111111</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1514,37 +1514,37 @@
         <v>34</v>
       </c>
       <c r="C24">
-        <v>234.55</v>
+        <v>241.58</v>
       </c>
       <c r="D24">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E24">
-        <v>0.4393790134098675</v>
+        <v>0.4536809108476315</v>
       </c>
       <c r="F24">
-        <v>0.7658730158730158</v>
+        <v>0.7876984126984127</v>
       </c>
       <c r="G24">
-        <v>0.277686504836311</v>
+        <v>0.2764922655972436</v>
       </c>
       <c r="H24">
-        <v>0.8988095238095238</v>
+        <v>0.8928571428571429</v>
       </c>
       <c r="I24">
-        <v>0.1861053352400992</v>
+        <v>0.1848024039268634</v>
       </c>
       <c r="J24">
         <v>0.9206349206349206</v>
       </c>
       <c r="K24">
-        <v>0.03937205203545157</v>
+        <v>0.03997204752391687</v>
       </c>
       <c r="L24">
-        <v>0.7976190476190476</v>
+        <v>0.8015873015873016</v>
       </c>
       <c r="M24">
-        <v>0.845734126984127</v>
+        <v>0.8506944444444444</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1555,37 +1555,37 @@
         <v>35</v>
       </c>
       <c r="C25">
-        <v>681.92</v>
+        <v>685.73</v>
       </c>
       <c r="D25">
         <v>28</v>
       </c>
       <c r="E25">
-        <v>0.5061131942186701</v>
+        <v>0.5183722594872799</v>
       </c>
       <c r="F25">
-        <v>0.8313492063492063</v>
+        <v>0.8412698412698413</v>
       </c>
       <c r="G25">
-        <v>0.2589501874437588</v>
+        <v>0.2691814415714111</v>
       </c>
       <c r="H25">
-        <v>0.875</v>
+        <v>0.8849206349206349</v>
       </c>
       <c r="I25">
-        <v>0.1296696516697254</v>
+        <v>0.1304551497619591</v>
       </c>
       <c r="J25">
-        <v>0.8214285714285714</v>
+        <v>0.8234126984126984</v>
       </c>
       <c r="K25">
-        <v>0.04819319679904804</v>
+        <v>0.0473609812647721</v>
       </c>
       <c r="L25">
-        <v>0.8551587301587301</v>
+        <v>0.8492063492063493</v>
       </c>
       <c r="M25">
-        <v>0.845734126984127</v>
+        <v>0.8497023809523809</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1596,37 +1596,37 @@
         <v>36</v>
       </c>
       <c r="C26">
-        <v>280.01</v>
+        <v>250.19</v>
       </c>
       <c r="D26">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E26">
-        <v>0.6004845610464798</v>
+        <v>0.5477336841308676</v>
       </c>
       <c r="F26">
-        <v>0.9027777777777777</v>
+        <v>0.8630952380952381</v>
       </c>
       <c r="G26">
-        <v>0.2380831273498086</v>
+        <v>0.3489154943606134</v>
       </c>
       <c r="H26">
-        <v>0.8333333333333333</v>
+        <v>0.9484126984126984</v>
       </c>
       <c r="I26">
-        <v>0.1710544285002033</v>
+        <v>0.1932104013249621</v>
       </c>
       <c r="J26">
-        <v>0.8928571428571429</v>
+        <v>0.9305555555555556</v>
       </c>
       <c r="K26">
-        <v>0.02347963027432792</v>
+        <v>0.002968569295497539</v>
       </c>
       <c r="L26">
-        <v>0.742063492063492</v>
+        <v>0.626984126984127</v>
       </c>
       <c r="M26">
-        <v>0.8427579365079365</v>
+        <v>0.8422619047619048</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1637,34 +1637,34 @@
         <v>37</v>
       </c>
       <c r="C27">
-        <v>463.2</v>
+        <v>448.6</v>
       </c>
       <c r="D27">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E27">
-        <v>0.4612152000380043</v>
+        <v>0.4658052174783746</v>
       </c>
       <c r="F27">
-        <v>0.7916666666666667</v>
+        <v>0.7956349206349206</v>
       </c>
       <c r="G27">
-        <v>0.2217875382823515</v>
+        <v>0.2177701572789685</v>
       </c>
       <c r="H27">
-        <v>0.8015873015873016</v>
+        <v>0.7956349206349206</v>
       </c>
       <c r="I27">
-        <v>0.1790989922874935</v>
+        <v>0.179611030195507</v>
       </c>
       <c r="J27">
         <v>0.9107142857142857</v>
       </c>
       <c r="K27">
-        <v>0.04919056800721536</v>
+        <v>0.05043106886061521</v>
       </c>
       <c r="L27">
-        <v>0.8571428571428571</v>
+        <v>0.8591269841269842</v>
       </c>
       <c r="M27">
         <v>0.8402777777777778</v>
@@ -1678,37 +1678,37 @@
         <v>38</v>
       </c>
       <c r="C28">
-        <v>256.78</v>
+        <v>277.07</v>
       </c>
       <c r="D28">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E28">
-        <v>0.5475065792052249</v>
+        <v>0.5877268437531821</v>
       </c>
       <c r="F28">
-        <v>0.8591269841269842</v>
+        <v>0.8908730158730158</v>
       </c>
       <c r="G28">
-        <v>0.3379929078871809</v>
+        <v>0.241689540424785</v>
       </c>
       <c r="H28">
-        <v>0.9424603174603174</v>
+        <v>0.8412698412698413</v>
       </c>
       <c r="I28">
-        <v>0.1934604490976719</v>
+        <v>0.1675149926699888</v>
       </c>
       <c r="J28">
-        <v>0.9305555555555556</v>
+        <v>0.882936507936508</v>
       </c>
       <c r="K28">
-        <v>0.002886997641083525</v>
+        <v>0.02405244680593918</v>
       </c>
       <c r="L28">
-        <v>0.626984126984127</v>
+        <v>0.742063492063492</v>
       </c>
       <c r="M28">
-        <v>0.839781746031746</v>
+        <v>0.8392857142857143</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -1719,37 +1719,37 @@
         <v>39</v>
       </c>
       <c r="C29">
-        <v>207.35</v>
+        <v>213.61</v>
       </c>
       <c r="D29">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E29">
-        <v>0.4384945978193247</v>
+        <v>0.4214939205896804</v>
       </c>
       <c r="F29">
-        <v>0.7599206349206349</v>
+        <v>0.75</v>
       </c>
       <c r="G29">
-        <v>0.2403635939185582</v>
+        <v>0.2461143354868384</v>
       </c>
       <c r="H29">
-        <v>0.8412698412698413</v>
+        <v>0.8492063492063493</v>
       </c>
       <c r="I29">
-        <v>0.2134998349885895</v>
+        <v>0.2128316603514803</v>
       </c>
       <c r="J29">
         <v>0.9404761904761905</v>
       </c>
       <c r="K29">
-        <v>0.03217096957068606</v>
+        <v>0.03217551287509884</v>
       </c>
       <c r="L29">
-        <v>0.7738095238095238</v>
+        <v>0.7718253968253969</v>
       </c>
       <c r="M29">
-        <v>0.8288690476190477</v>
+        <v>0.8278769841269842</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -1760,37 +1760,37 @@
         <v>40</v>
       </c>
       <c r="C30">
-        <v>342.85</v>
+        <v>85.42</v>
       </c>
       <c r="D30">
-        <v>57</v>
+        <v>229</v>
       </c>
       <c r="E30">
-        <v>0.4219177667287918</v>
+        <v>0.3692752941497895</v>
       </c>
       <c r="F30">
-        <v>0.751984126984127</v>
+        <v>0.6865079365079364</v>
       </c>
       <c r="G30">
-        <v>0.2859730829687234</v>
+        <v>0.1584317902331342</v>
       </c>
       <c r="H30">
-        <v>0.9107142857142857</v>
+        <v>0.6765873015873016</v>
       </c>
       <c r="I30">
-        <v>0.1669877762264658</v>
+        <v>0.2937644977594535</v>
       </c>
       <c r="J30">
-        <v>0.8849206349206349</v>
+        <v>0.9781746031746031</v>
       </c>
       <c r="K30">
-        <v>0.029750027473134</v>
+        <v>0.1024534398035731</v>
       </c>
       <c r="L30">
-        <v>0.7658730158730158</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="M30">
-        <v>0.8283730158730158</v>
+        <v>0.8263888888888888</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -1801,37 +1801,37 @@
         <v>41</v>
       </c>
       <c r="C31">
-        <v>67.27</v>
+        <v>66.2</v>
       </c>
       <c r="D31">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="E31">
-        <v>0.4577283496065238</v>
+        <v>0.4499124248929512</v>
       </c>
       <c r="F31">
-        <v>0.7876984126984127</v>
+        <v>0.7797619047619048</v>
       </c>
       <c r="G31">
-        <v>0.276244139763681</v>
+        <v>0.283076263861194</v>
       </c>
       <c r="H31">
-        <v>0.8948412698412699</v>
+        <v>0.9027777777777777</v>
       </c>
       <c r="I31">
-        <v>0.1615929329166995</v>
+        <v>0.1580624257840973</v>
       </c>
       <c r="J31">
-        <v>0.871031746031746</v>
+        <v>0.8630952380952381</v>
       </c>
       <c r="K31">
-        <v>0.0274212847532416</v>
+        <v>0.02709068157897541</v>
       </c>
       <c r="L31">
         <v>0.755952380952381</v>
       </c>
       <c r="M31">
-        <v>0.8273809523809524</v>
+        <v>0.8253968253968254</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -1842,37 +1842,37 @@
         <v>42</v>
       </c>
       <c r="C32">
-        <v>86.67</v>
+        <v>350.44</v>
       </c>
       <c r="D32">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="E32">
-        <v>0.3638330383686301</v>
+        <v>0.4222268923921404</v>
       </c>
       <c r="F32">
-        <v>0.6805555555555556</v>
+        <v>0.751984126984127</v>
       </c>
       <c r="G32">
-        <v>0.1588685564794437</v>
+        <v>0.2846833419457594</v>
       </c>
       <c r="H32">
-        <v>0.6785714285714286</v>
+        <v>0.9067460317460317</v>
       </c>
       <c r="I32">
-        <v>0.2933666475421793</v>
+        <v>0.1620521482687564</v>
       </c>
       <c r="J32">
-        <v>0.9781746031746031</v>
+        <v>0.871031746031746</v>
       </c>
       <c r="K32">
-        <v>0.104989560621964</v>
+        <v>0.030472865555597</v>
       </c>
       <c r="L32">
-        <v>0.9662698412698413</v>
+        <v>0.7678571428571429</v>
       </c>
       <c r="M32">
-        <v>0.8258928571428572</v>
+        <v>0.8244047619047619</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -1883,37 +1883,37 @@
         <v>43</v>
       </c>
       <c r="C33">
-        <v>99.92</v>
+        <v>83.93000000000001</v>
       </c>
       <c r="D33">
-        <v>196</v>
+        <v>233</v>
       </c>
       <c r="E33">
-        <v>0.5280216507464104</v>
+        <v>0.6262025082416323</v>
       </c>
       <c r="F33">
-        <v>0.8472222222222223</v>
+        <v>0.9206349206349206</v>
       </c>
       <c r="G33">
-        <v>0.2846516241143491</v>
+        <v>0.1992083307734406</v>
       </c>
       <c r="H33">
-        <v>0.9087301587301587</v>
+        <v>0.7678571428571429</v>
       </c>
       <c r="I33">
-        <v>0.124355632043659</v>
+        <v>0.1844029069686499</v>
       </c>
       <c r="J33">
-        <v>0.8174603174603174</v>
+        <v>0.9166666666666667</v>
       </c>
       <c r="K33">
-        <v>0.02128569537092544</v>
+        <v>0.01534025584003132</v>
       </c>
       <c r="L33">
-        <v>0.7202380952380952</v>
+        <v>0.6884920634920636</v>
       </c>
       <c r="M33">
-        <v>0.8234126984126984</v>
+        <v>0.8234126984126985</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1924,37 +1924,37 @@
         <v>44</v>
       </c>
       <c r="C34">
-        <v>84.88</v>
+        <v>200.8</v>
       </c>
       <c r="D34">
-        <v>231</v>
+        <v>97</v>
       </c>
       <c r="E34">
-        <v>0.6268713855631995</v>
+        <v>0.5606762231899484</v>
       </c>
       <c r="F34">
-        <v>0.9166666666666667</v>
+        <v>0.871031746031746</v>
       </c>
       <c r="G34">
-        <v>0.1953652704370877</v>
+        <v>0.3417208894397377</v>
       </c>
       <c r="H34">
-        <v>0.757936507936508</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="I34">
-        <v>0.1881150424267935</v>
+        <v>0.1130992703600745</v>
       </c>
       <c r="J34">
-        <v>0.9265873015873016</v>
+        <v>0.7916666666666667</v>
       </c>
       <c r="K34">
-        <v>0.01545803208134017</v>
+        <v>0.01530606621327603</v>
       </c>
       <c r="L34">
-        <v>0.6884920634920636</v>
+        <v>0.6865079365079364</v>
       </c>
       <c r="M34">
-        <v>0.822420634920635</v>
+        <v>0.8234126984126984</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -1965,37 +1965,37 @@
         <v>45</v>
       </c>
       <c r="C35">
-        <v>199.9</v>
+        <v>99.16</v>
       </c>
       <c r="D35">
-        <v>98</v>
+        <v>197</v>
       </c>
       <c r="E35">
-        <v>0.5450913666516796</v>
+        <v>0.5256124263954027</v>
       </c>
       <c r="F35">
-        <v>0.8571428571428571</v>
+        <v>0.8472222222222223</v>
       </c>
       <c r="G35">
-        <v>0.352728488228183</v>
+        <v>0.2830046207818269</v>
       </c>
       <c r="H35">
-        <v>0.9484126984126984</v>
+        <v>0.9007936507936507</v>
       </c>
       <c r="I35">
-        <v>0.1132213642286946</v>
+        <v>0.1257477255403154</v>
       </c>
       <c r="J35">
-        <v>0.7837301587301587</v>
+        <v>0.8154761904761905</v>
       </c>
       <c r="K35">
-        <v>0.01540841323476305</v>
+        <v>0.02079486438924693</v>
       </c>
       <c r="L35">
-        <v>0.6865079365079364</v>
+        <v>0.7182539682539683</v>
       </c>
       <c r="M35">
-        <v>0.8189484126984127</v>
+        <v>0.8204365079365079</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2006,37 +2006,37 @@
         <v>46</v>
       </c>
       <c r="C36">
-        <v>67.20999999999999</v>
+        <v>65.61</v>
       </c>
       <c r="D36">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="E36">
-        <v>0.7809914470561584</v>
+        <v>0.7723629235947381</v>
       </c>
       <c r="F36">
         <v>0.9662698412698413</v>
       </c>
       <c r="G36">
-        <v>0.3549950565357624</v>
+        <v>0.354250944118109</v>
       </c>
       <c r="H36">
-        <v>0.9523809523809524</v>
+        <v>0.9503968253968255</v>
       </c>
       <c r="I36">
-        <v>0.340046226107403</v>
+        <v>0.3364630946191979</v>
       </c>
       <c r="J36">
-        <v>0.9861111111111112</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="K36">
-        <v>-0.04124067272166905</v>
+        <v>-0.04147093490024455</v>
       </c>
       <c r="L36">
-        <v>0.3670634920634921</v>
+        <v>0.3650793650793651</v>
       </c>
       <c r="M36">
-        <v>0.8179563492063493</v>
+        <v>0.8159722222222222</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2047,34 +2047,34 @@
         <v>47</v>
       </c>
       <c r="C37">
-        <v>351.08</v>
+        <v>355.94</v>
       </c>
       <c r="D37">
         <v>55</v>
       </c>
       <c r="E37">
-        <v>0.7214759192844874</v>
+        <v>0.7185077969116737</v>
       </c>
       <c r="F37">
-        <v>0.9603174603174603</v>
+        <v>0.9563492063492063</v>
       </c>
       <c r="G37">
-        <v>0.3934739174645047</v>
+        <v>0.3932343904227443</v>
       </c>
       <c r="H37">
         <v>0.9702380952380952</v>
       </c>
       <c r="I37">
-        <v>0.1776773269785799</v>
+        <v>0.1773936787440921</v>
       </c>
       <c r="J37">
         <v>0.9047619047619048</v>
       </c>
       <c r="K37">
-        <v>-0.03210668993980388</v>
+        <v>-0.03255018162422722</v>
       </c>
       <c r="L37">
-        <v>0.4186507936507937</v>
+        <v>0.4226190476190476</v>
       </c>
       <c r="M37">
         <v>0.8134920634920635</v>
@@ -2088,37 +2088,37 @@
         <v>48</v>
       </c>
       <c r="C38">
-        <v>159.94</v>
+        <v>156.67</v>
       </c>
       <c r="D38">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E38">
-        <v>0.3087603911354042</v>
+        <v>0.3042168025788231</v>
       </c>
       <c r="F38">
-        <v>0.5992063492063492</v>
+        <v>0.5853174603174603</v>
       </c>
       <c r="G38">
-        <v>0.2649630188730214</v>
+        <v>0.2625561797594858</v>
       </c>
       <c r="H38">
-        <v>0.880952380952381</v>
+        <v>0.873015873015873</v>
       </c>
       <c r="I38">
-        <v>0.290813214611033</v>
+        <v>0.2925799383910566</v>
       </c>
       <c r="J38">
         <v>0.9761904761904762</v>
       </c>
       <c r="K38">
-        <v>0.03796214853974145</v>
+        <v>0.03764149176006983</v>
       </c>
       <c r="L38">
         <v>0.7916666666666667</v>
       </c>
       <c r="M38">
-        <v>0.8120039682539683</v>
+        <v>0.8065476190476191</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2129,37 +2129,37 @@
         <v>49</v>
       </c>
       <c r="C39">
-        <v>58.55</v>
+        <v>130.08</v>
       </c>
       <c r="D39">
-        <v>334</v>
+        <v>150</v>
       </c>
       <c r="E39">
-        <v>0.6427551318196738</v>
+        <v>0.3080045933056527</v>
       </c>
       <c r="F39">
-        <v>0.9285714285714286</v>
+        <v>0.5932539682539683</v>
       </c>
       <c r="G39">
-        <v>0.2275318555126593</v>
+        <v>0.1750207379692004</v>
       </c>
       <c r="H39">
-        <v>0.8154761904761905</v>
+        <v>0.7083333333333333</v>
       </c>
       <c r="I39">
-        <v>0.1018717006808386</v>
+        <v>0.2178363896149118</v>
       </c>
       <c r="J39">
-        <v>0.744047619047619</v>
+        <v>0.9484126984126984</v>
       </c>
       <c r="K39">
-        <v>0.02315458166976637</v>
+        <v>0.1083508154343995</v>
       </c>
       <c r="L39">
-        <v>0.7400793650793651</v>
+        <v>0.9682539682539683</v>
       </c>
       <c r="M39">
-        <v>0.8070436507936508</v>
+        <v>0.8045634920634921</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2170,37 +2170,37 @@
         <v>50</v>
       </c>
       <c r="C40">
-        <v>335.2</v>
+        <v>344.87</v>
       </c>
       <c r="D40">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E40">
-        <v>1.328553433518397</v>
+        <v>1.324889286187718</v>
       </c>
       <c r="F40">
-        <v>0.996031746031746</v>
+        <v>0.994047619047619</v>
       </c>
       <c r="G40">
-        <v>0.4499976433802351</v>
+        <v>0.4438337516782769</v>
       </c>
       <c r="H40">
-        <v>0.9781746031746031</v>
+        <v>0.9761904761904762</v>
       </c>
       <c r="I40">
-        <v>0.1199755585626561</v>
+        <v>0.1154460687336415</v>
       </c>
       <c r="J40">
-        <v>0.8015873015873016</v>
+        <v>0.7976190476190476</v>
       </c>
       <c r="K40">
-        <v>-0.02949407725815212</v>
+        <v>-0.02857269284596706</v>
       </c>
       <c r="L40">
-        <v>0.4384920634920635</v>
+        <v>0.4424603174603174</v>
       </c>
       <c r="M40">
-        <v>0.8035714285714286</v>
+        <v>0.802579365079365</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2211,37 +2211,37 @@
         <v>51</v>
       </c>
       <c r="C41">
-        <v>45.2</v>
+        <v>59.03</v>
       </c>
       <c r="D41">
-        <v>433</v>
+        <v>332</v>
       </c>
       <c r="E41">
-        <v>0.4968247504498049</v>
+        <v>0.6202089437677122</v>
       </c>
       <c r="F41">
-        <v>0.8214285714285714</v>
+        <v>0.9126984126984127</v>
       </c>
       <c r="G41">
-        <v>0.1734101980031223</v>
+        <v>0.2286950902111796</v>
       </c>
       <c r="H41">
-        <v>0.7003968253968255</v>
+        <v>0.8174603174603174</v>
       </c>
       <c r="I41">
-        <v>0.1019174195843151</v>
+        <v>0.1007569963717855</v>
       </c>
       <c r="J41">
-        <v>0.746031746031746</v>
+        <v>0.7400793650793651</v>
       </c>
       <c r="K41">
-        <v>0.0825892430253026</v>
+        <v>0.02269822476090085</v>
       </c>
       <c r="L41">
-        <v>0.9325396825396826</v>
+        <v>0.7341269841269842</v>
       </c>
       <c r="M41">
-        <v>0.8000992063492064</v>
+        <v>0.8010912698412699</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2252,37 +2252,37 @@
         <v>52</v>
       </c>
       <c r="C42">
-        <v>134.93</v>
+        <v>45.29</v>
       </c>
       <c r="D42">
-        <v>145</v>
+        <v>432</v>
       </c>
       <c r="E42">
-        <v>0.2998856641128533</v>
+        <v>0.4883063812873064</v>
       </c>
       <c r="F42">
-        <v>0.5813492063492063</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="G42">
-        <v>0.1728501733462456</v>
+        <v>0.1695828997237968</v>
       </c>
       <c r="H42">
         <v>0.6984126984126984</v>
       </c>
       <c r="I42">
-        <v>0.2197695984478189</v>
+        <v>0.1007857039343941</v>
       </c>
       <c r="J42">
-        <v>0.9444444444444444</v>
+        <v>0.742063492063492</v>
       </c>
       <c r="K42">
-        <v>0.1082154244442324</v>
+        <v>0.0830060421752821</v>
       </c>
       <c r="L42">
-        <v>0.9702380952380952</v>
+        <v>0.9365079365079364</v>
       </c>
       <c r="M42">
-        <v>0.798611111111111</v>
+        <v>0.7991071428571428</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2293,31 +2293,31 @@
         <v>53</v>
       </c>
       <c r="C43">
-        <v>238.48</v>
+        <v>237.96</v>
       </c>
       <c r="D43">
         <v>82</v>
       </c>
       <c r="E43">
-        <v>0.361038328717655</v>
+        <v>0.362161618456683</v>
       </c>
       <c r="F43">
         <v>0.6746031746031745</v>
       </c>
       <c r="G43">
-        <v>0.2748113086963195</v>
+        <v>0.2768987189938698</v>
       </c>
       <c r="H43">
-        <v>0.8928571428571429</v>
+        <v>0.8948412698412699</v>
       </c>
       <c r="I43">
-        <v>0.128662746245345</v>
+        <v>0.1258525558203467</v>
       </c>
       <c r="J43">
-        <v>0.8194444444444444</v>
+        <v>0.8174603174603174</v>
       </c>
       <c r="K43">
-        <v>0.03699485870440333</v>
+        <v>0.03660674848518439</v>
       </c>
       <c r="L43">
         <v>0.7896825396825397</v>
@@ -2334,37 +2334,37 @@
         <v>54</v>
       </c>
       <c r="C44">
-        <v>74.38</v>
+        <v>40.6</v>
       </c>
       <c r="D44">
-        <v>263</v>
+        <v>482</v>
       </c>
       <c r="E44">
-        <v>0.5762077647557051</v>
+        <v>1.6586745451858</v>
       </c>
       <c r="F44">
-        <v>0.880952380952381</v>
+        <v>1</v>
       </c>
       <c r="G44">
-        <v>0.2303238797862049</v>
+        <v>0.516761291187574</v>
       </c>
       <c r="H44">
-        <v>0.8214285714285714</v>
+        <v>0.992063492063492</v>
       </c>
       <c r="I44">
-        <v>0.1143565154802293</v>
+        <v>0.3454331307296893</v>
       </c>
       <c r="J44">
-        <v>0.7896825396825397</v>
+        <v>0.9900793650793651</v>
       </c>
       <c r="K44">
-        <v>0.0151689186660284</v>
+        <v>-0.0790116529400368</v>
       </c>
       <c r="L44">
-        <v>0.6825396825396826</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="M44">
-        <v>0.7936507936507937</v>
+        <v>0.7901785714285714</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2375,34 +2375,34 @@
         <v>55</v>
       </c>
       <c r="C45">
-        <v>626.72</v>
+        <v>73.05</v>
       </c>
       <c r="D45">
-        <v>31</v>
+        <v>268</v>
       </c>
       <c r="E45">
-        <v>0.6529103208109314</v>
+        <v>0.5698779290402629</v>
       </c>
       <c r="F45">
-        <v>0.9345238095238095</v>
+        <v>0.878968253968254</v>
       </c>
       <c r="G45">
-        <v>0.3199709914148837</v>
+        <v>0.2283541091707664</v>
       </c>
       <c r="H45">
-        <v>0.9325396825396826</v>
+        <v>0.8154761904761905</v>
       </c>
       <c r="I45">
-        <v>0.1060705666647543</v>
+        <v>0.1105370878561481</v>
       </c>
       <c r="J45">
-        <v>0.7678571428571429</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="K45">
-        <v>-0.01439542332545844</v>
+        <v>0.0153046288873539</v>
       </c>
       <c r="L45">
-        <v>0.5218253968253969</v>
+        <v>0.6845238095238095</v>
       </c>
       <c r="M45">
         <v>0.7891865079365079</v>
@@ -2416,37 +2416,37 @@
         <v>56</v>
       </c>
       <c r="C46">
-        <v>41.1</v>
+        <v>622.77</v>
       </c>
       <c r="D46">
-        <v>477</v>
+        <v>31</v>
       </c>
       <c r="E46">
-        <v>1.64424252245809</v>
+        <v>0.6453841540359062</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0.9305555555555556</v>
       </c>
       <c r="G46">
-        <v>0.524347426679299</v>
+        <v>0.327381995511259</v>
       </c>
       <c r="H46">
-        <v>0.992063492063492</v>
+        <v>0.9345238095238095</v>
       </c>
       <c r="I46">
-        <v>0.3490257928204749</v>
+        <v>0.1058358947781648</v>
       </c>
       <c r="J46">
-        <v>0.9900793650793651</v>
+        <v>0.7638888888888888</v>
       </c>
       <c r="K46">
-        <v>-0.08099598526012169</v>
+        <v>-0.01383626250325082</v>
       </c>
       <c r="L46">
-        <v>0.1746031746031746</v>
+        <v>0.5238095238095238</v>
       </c>
       <c r="M46">
-        <v>0.7891865079365079</v>
+        <v>0.7881944444444444</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2457,37 +2457,37 @@
         <v>57</v>
       </c>
       <c r="C47">
-        <v>271.57</v>
+        <v>269.83</v>
       </c>
       <c r="D47">
         <v>72</v>
       </c>
       <c r="E47">
-        <v>0.5652185813755058</v>
+        <v>0.5430342607326644</v>
       </c>
       <c r="F47">
-        <v>0.875</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="G47">
-        <v>0.2622193324290469</v>
+        <v>0.2686528796816967</v>
       </c>
       <c r="H47">
-        <v>0.878968253968254</v>
+        <v>0.882936507936508</v>
       </c>
       <c r="I47">
-        <v>0.0991608891190144</v>
+        <v>0.0975061403868199</v>
       </c>
       <c r="J47">
-        <v>0.7301587301587301</v>
+        <v>0.7321428571428571</v>
       </c>
       <c r="K47">
-        <v>0.01058961261442238</v>
+        <v>0.01077169861784742</v>
       </c>
       <c r="L47">
         <v>0.6626984126984127</v>
       </c>
       <c r="M47">
-        <v>0.7867063492063492</v>
+        <v>0.7837301587301587</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2498,37 +2498,37 @@
         <v>58</v>
       </c>
       <c r="C48">
-        <v>5708.39</v>
+        <v>138.03</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>142</v>
       </c>
       <c r="E48">
-        <v>0.3485899627318076</v>
+        <v>0.22832724670749</v>
       </c>
       <c r="F48">
-        <v>0.6488095238095238</v>
+        <v>0.4841269841269841</v>
       </c>
       <c r="G48">
-        <v>0.1838058461479395</v>
+        <v>0.3743865008341786</v>
       </c>
       <c r="H48">
-        <v>0.7321428571428571</v>
+        <v>0.9603174603174603</v>
       </c>
       <c r="I48">
-        <v>0.1144575996128889</v>
+        <v>0.5358059257659797</v>
       </c>
       <c r="J48">
-        <v>0.7916666666666667</v>
+        <v>0.998015873015873</v>
       </c>
       <c r="K48">
-        <v>0.10394260372271</v>
+        <v>0.01553377016062851</v>
       </c>
       <c r="L48">
-        <v>0.9642857142857143</v>
+        <v>0.6904761904761905</v>
       </c>
       <c r="M48">
-        <v>0.7842261904761905</v>
+        <v>0.783234126984127</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -2539,37 +2539,37 @@
         <v>59</v>
       </c>
       <c r="C49">
-        <v>670.26</v>
+        <v>669.28</v>
       </c>
       <c r="D49">
         <v>29</v>
       </c>
       <c r="E49">
-        <v>0.4133443462710972</v>
+        <v>0.4083109975020154</v>
       </c>
       <c r="F49">
-        <v>0.742063492063492</v>
+        <v>0.7380952380952381</v>
       </c>
       <c r="G49">
-        <v>0.3596236051075936</v>
+        <v>0.365679416381157</v>
       </c>
       <c r="H49">
         <v>0.9543650793650794</v>
       </c>
       <c r="I49">
-        <v>0.09268600400922926</v>
+        <v>0.09346501395392749</v>
       </c>
       <c r="J49">
         <v>0.7083333333333333</v>
       </c>
       <c r="K49">
-        <v>0.02238373452225384</v>
+        <v>0.02184849003174069</v>
       </c>
       <c r="L49">
-        <v>0.7301587301587301</v>
+        <v>0.7281746031746031</v>
       </c>
       <c r="M49">
-        <v>0.7837301587301587</v>
+        <v>0.7822420634920635</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -2580,37 +2580,37 @@
         <v>60</v>
       </c>
       <c r="C50">
-        <v>141.6</v>
+        <v>5681.29</v>
       </c>
       <c r="D50">
-        <v>138</v>
+        <v>3</v>
       </c>
       <c r="E50">
-        <v>0.227697087401815</v>
+        <v>0.3376769914267252</v>
       </c>
       <c r="F50">
-        <v>0.4841269841269841</v>
+        <v>0.6349206349206349</v>
       </c>
       <c r="G50">
-        <v>0.3699070008310632</v>
+        <v>0.1865057582812744</v>
       </c>
       <c r="H50">
-        <v>0.9583333333333333</v>
+        <v>0.7361111111111112</v>
       </c>
       <c r="I50">
-        <v>0.5423006937125382</v>
+        <v>0.111772348706708</v>
       </c>
       <c r="J50">
-        <v>0.998015873015873</v>
+        <v>0.7857142857142857</v>
       </c>
       <c r="K50">
-        <v>0.01618234952261782</v>
+        <v>0.1034604582701674</v>
       </c>
       <c r="L50">
-        <v>0.6944444444444444</v>
+        <v>0.9662698412698413</v>
       </c>
       <c r="M50">
-        <v>0.7837301587301587</v>
+        <v>0.7807539682539683</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -2621,37 +2621,37 @@
         <v>61</v>
       </c>
       <c r="C51">
-        <v>83.05</v>
+        <v>84.31999999999999</v>
       </c>
       <c r="D51">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E51">
-        <v>0.4962685454986173</v>
+        <v>0.485856444542377</v>
       </c>
       <c r="F51">
-        <v>0.8194444444444444</v>
+        <v>0.8154761904761905</v>
       </c>
       <c r="G51">
-        <v>0.2381646524320674</v>
+        <v>0.238049874249437</v>
       </c>
       <c r="H51">
-        <v>0.8353174603174603</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="I51">
-        <v>0.2481821003397825</v>
+        <v>0.2469929914408436</v>
       </c>
       <c r="J51">
         <v>0.9563492063492063</v>
       </c>
       <c r="K51">
-        <v>-0.0176437742006519</v>
+        <v>-0.01701283425965677</v>
       </c>
       <c r="L51">
         <v>0.5099206349206349</v>
       </c>
       <c r="M51">
-        <v>0.7802579365079365</v>
+        <v>0.7787698412698412</v>
       </c>
     </row>
     <row r="52" spans="1:13">
@@ -2662,37 +2662,37 @@
         <v>62</v>
       </c>
       <c r="C52">
-        <v>243.49</v>
+        <v>228.89</v>
       </c>
       <c r="D52">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E52">
-        <v>0.4896154459278139</v>
+        <v>0.5827739473813959</v>
       </c>
       <c r="F52">
-        <v>0.8095238095238095</v>
+        <v>0.8869047619047619</v>
       </c>
       <c r="G52">
-        <v>0.2231169472655087</v>
+        <v>0.336567690329686</v>
       </c>
       <c r="H52">
-        <v>0.8035714285714286</v>
+        <v>0.9404761904761905</v>
       </c>
       <c r="I52">
-        <v>0.137482081867712</v>
+        <v>0.09726396315442827</v>
       </c>
       <c r="J52">
-        <v>0.8392857142857143</v>
+        <v>0.7281746031746031</v>
       </c>
       <c r="K52">
-        <v>0.008167593935080902</v>
+        <v>-0.009194071153570431</v>
       </c>
       <c r="L52">
-        <v>0.6507936507936507</v>
+        <v>0.5515873015873016</v>
       </c>
       <c r="M52">
-        <v>0.7757936507936508</v>
+        <v>0.7767857142857143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>